<commit_message>
Feat : GA Algorithm done
</commit_message>
<xml_diff>
--- a/backend/datas/openedclass/S1IF_updated.xlsx
+++ b/backend/datas/openedclass/S1IF_updated.xlsx
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="P3" t="n">
-        <v>1007</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4">
@@ -1828,7 +1828,7 @@
         </is>
       </c>
       <c r="P20" t="n">
-        <v>1008</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21">
@@ -2040,7 +2040,7 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>1007</v>
+        <v>210</v>
       </c>
     </row>
     <row r="24">
@@ -4384,7 +4384,7 @@
         </is>
       </c>
       <c r="P57" t="n">
-        <v>1009</v>
+        <v>212</v>
       </c>
     </row>
     <row r="58">
@@ -4452,7 +4452,7 @@
         </is>
       </c>
       <c r="P58" t="n">
-        <v>1010</v>
+        <v>213</v>
       </c>
     </row>
     <row r="59">
@@ -4524,7 +4524,7 @@
         </is>
       </c>
       <c r="P59" t="n">
-        <v>1009</v>
+        <v>212</v>
       </c>
     </row>
     <row r="60">
@@ -4592,7 +4592,7 @@
         </is>
       </c>
       <c r="P60" t="n">
-        <v>1011</v>
+        <v>214</v>
       </c>
     </row>
     <row r="61">
@@ -4664,7 +4664,7 @@
         </is>
       </c>
       <c r="P61" t="n">
-        <v>1009</v>
+        <v>212</v>
       </c>
     </row>
     <row r="62">
@@ -5840,7 +5840,7 @@
         </is>
       </c>
       <c r="P78" t="n">
-        <v>1011</v>
+        <v>214</v>
       </c>
     </row>
     <row r="79">
@@ -5912,7 +5912,7 @@
         </is>
       </c>
       <c r="P79" t="n">
-        <v>1009</v>
+        <v>212</v>
       </c>
     </row>
     <row r="80">
@@ -5980,7 +5980,7 @@
         </is>
       </c>
       <c r="P80" t="n">
-        <v>1010</v>
+        <v>213</v>
       </c>
     </row>
     <row r="81">
@@ -6052,7 +6052,7 @@
         </is>
       </c>
       <c r="P81" t="n">
-        <v>1009</v>
+        <v>212</v>
       </c>
     </row>
     <row r="82">
@@ -8880,7 +8880,7 @@
         </is>
       </c>
       <c r="P122" t="n">
-        <v>1012</v>
+        <v>215</v>
       </c>
     </row>
     <row r="123">
@@ -8948,7 +8948,7 @@
       </c>
       <c r="O123" t="inlineStr"/>
       <c r="P123" t="n">
-        <v>1013</v>
+        <v>216</v>
       </c>
     </row>
     <row r="124">
@@ -9016,7 +9016,7 @@
         </is>
       </c>
       <c r="P124" t="n">
-        <v>1014</v>
+        <v>217</v>
       </c>
     </row>
     <row r="125">
@@ -9084,7 +9084,7 @@
       </c>
       <c r="O125" t="inlineStr"/>
       <c r="P125" t="n">
-        <v>1013</v>
+        <v>216</v>
       </c>
     </row>
     <row r="126">
@@ -9152,7 +9152,7 @@
         </is>
       </c>
       <c r="P126" t="n">
-        <v>1015</v>
+        <v>218</v>
       </c>
     </row>
     <row r="127">
@@ -9220,7 +9220,7 @@
       </c>
       <c r="O127" t="inlineStr"/>
       <c r="P127" t="n">
-        <v>1013</v>
+        <v>216</v>
       </c>
     </row>
     <row r="128">
@@ -9628,7 +9628,7 @@
         </is>
       </c>
       <c r="P133" t="n">
-        <v>1012</v>
+        <v>215</v>
       </c>
     </row>
     <row r="134">
@@ -9696,7 +9696,7 @@
       </c>
       <c r="O134" t="inlineStr"/>
       <c r="P134" t="n">
-        <v>1013</v>
+        <v>216</v>
       </c>
     </row>
     <row r="135">
@@ -9764,7 +9764,7 @@
         </is>
       </c>
       <c r="P135" t="n">
-        <v>1014</v>
+        <v>217</v>
       </c>
     </row>
     <row r="136">
@@ -9832,7 +9832,7 @@
       </c>
       <c r="O136" t="inlineStr"/>
       <c r="P136" t="n">
-        <v>1013</v>
+        <v>216</v>
       </c>
     </row>
     <row r="137">
@@ -11012,7 +11012,7 @@
         </is>
       </c>
       <c r="P153" t="n">
-        <v>1004</v>
+        <v>207</v>
       </c>
     </row>
     <row r="154">
@@ -11080,7 +11080,7 @@
         </is>
       </c>
       <c r="P154" t="n">
-        <v>1005</v>
+        <v>208</v>
       </c>
     </row>
     <row r="155">
@@ -12324,7 +12324,7 @@
         </is>
       </c>
       <c r="P172" t="n">
-        <v>1016</v>
+        <v>219</v>
       </c>
     </row>
     <row r="173">
@@ -12896,7 +12896,7 @@
         </is>
       </c>
       <c r="P180" t="n">
-        <v>1003</v>
+        <v>206</v>
       </c>
     </row>
     <row r="181">
@@ -13108,7 +13108,7 @@
         </is>
       </c>
       <c r="P183" t="n">
-        <v>1003</v>
+        <v>206</v>
       </c>
     </row>
     <row r="184">
@@ -13520,7 +13520,7 @@
         </is>
       </c>
       <c r="P189" t="n">
-        <v>1003</v>
+        <v>206</v>
       </c>
     </row>
     <row r="190">
@@ -13800,7 +13800,7 @@
         </is>
       </c>
       <c r="P193" t="n">
-        <v>1003</v>
+        <v>206</v>
       </c>
     </row>
     <row r="194">
@@ -13940,7 +13940,7 @@
         </is>
       </c>
       <c r="P195" t="n">
-        <v>1003</v>
+        <v>206</v>
       </c>
     </row>
     <row r="196">
@@ -14768,7 +14768,7 @@
         </is>
       </c>
       <c r="P207" t="n">
-        <v>1003</v>
+        <v>206</v>
       </c>
     </row>
     <row r="208">

</xml_diff>